<commit_message>
Updated arrays negative scenarios
</commit_message>
<xml_diff>
--- a/src/test/resources/Exceldata/Login.xlsx
+++ b/src/test/resources/Exceldata/Login.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vanis\eclipse-numpyninja\DS-ALGO\src\test\resources\Exceldata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{147DEED8-05A3-4242-AB80-0EB09BE73991}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF600EC-989F-435F-BF4B-B0451BADE992}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -501,7 +501,7 @@
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>

</xml_diff>